<commit_message>
Various UI improvements based on feedback
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/SUGAR Unity Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/SUGAR Unity Localization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
   <si>
     <t>Key</t>
   </si>
@@ -266,13 +266,25 @@
   </si>
   <si>
     <t>Error: Unable to gather list of group members.</t>
+  </si>
+  <si>
+    <t>Risultati</t>
+  </si>
+  <si>
+    <t>Classifiche</t>
+  </si>
+  <si>
+    <t>Avanti</t>
+  </si>
+  <si>
+    <t>Precedente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -285,6 +297,17 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -307,10 +330,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +643,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -649,15 +674,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
+      <c r="C3" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -783,10 +808,10 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -794,10 +819,10 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -825,15 +850,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
+      <c r="C19" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -869,15 +894,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>5</v>
+      <c r="C23" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -959,10 +984,10 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>5</v>
@@ -970,54 +995,54 @@
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>5</v>
+      <c r="C33" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>5</v>
@@ -1025,10 +1050,10 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>5</v>
@@ -1036,10 +1061,10 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>5</v>
@@ -1047,10 +1072,10 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>5</v>
@@ -1058,10 +1083,10 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>5</v>
@@ -1069,16 +1094,20 @@
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:C41">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>